<commit_message>
Einzele Wörter in Splate erkennen
</commit_message>
<xml_diff>
--- a/Example/example.xlsx
+++ b/Example/example.xlsx
@@ -35,10 +35,10 @@
     <t xml:space="preserve">27.05. Tegel-Munich 1200-1400</t>
   </si>
   <si>
-    <t xml:space="preserve">DFA,DA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Berlin</t>
+    <t xml:space="preserve">DFA, DA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Berlin, TXL</t>
   </si>
 </sst>
 </file>
@@ -144,12 +144,12 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="35.9234693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Größere Zeilen können verglichen werden
</commit_message>
<xml_diff>
--- a/Example/example.xlsx
+++ b/Example/example.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t xml:space="preserve">Abkürzungen</t>
   </si>
@@ -35,10 +35,13 @@
     <t xml:space="preserve">27.05. Tegel-Munich 1200-1400</t>
   </si>
   <si>
-    <t xml:space="preserve">DFA, DA</t>
-  </si>
-  <si>
     <t xml:space="preserve">Berlin, TXL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DFA, Düsseldorf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADF</t>
   </si>
 </sst>
 </file>
@@ -139,17 +142,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="35.9234693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="38.4285714285714"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -161,6 +164,9 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="0" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -174,17 +180,17 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>